<commit_message>
Changes in dashboard file
</commit_message>
<xml_diff>
--- a/docs/Formats.xlsx
+++ b/docs/Formats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://interpublic-my.sharepoint.com/personal/ishank_aggarwal_interactiveavenues_com/Documents/Documents/Amazon/1. Report Automation/App/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{AC4A6378-67D2-4863-A478-442891091073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{114877BA-9867-4570-8DD2-AEADA8B4F5C7}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{AC4A6378-67D2-4863-A478-442891091073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF0A910A-6BE2-4608-BCA3-1AAACEE62081}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="30" windowWidth="14880" windowHeight="8520" xr2:uid="{0E2EABC8-826B-4772-8AE8-49EDCC4016C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0E2EABC8-826B-4772-8AE8-49EDCC4016C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Beauty" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="270">
   <si>
     <t>DailyHunt</t>
   </si>
@@ -836,6 +836,18 @@
   </si>
   <si>
     <t>NoBrokerHood</t>
+  </si>
+  <si>
+    <t>Viads</t>
+  </si>
+  <si>
+    <t>ApnaComplex</t>
+  </si>
+  <si>
+    <t>SportsKeeda</t>
+  </si>
+  <si>
+    <t>PublicApp</t>
   </si>
 </sst>
 </file>
@@ -1512,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A87D61-9DF9-4A12-B690-8C861BD071FC}">
-  <dimension ref="A1:CK30"/>
+  <dimension ref="A1:CN30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CE1" zoomScale="66" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="CO8" sqref="CO8"/>
+    <sheetView tabSelected="1" topLeftCell="BK1" zoomScale="66" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BT2" sqref="BT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1567,7 +1579,7 @@
     <col min="84" max="84" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:92" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>83</v>
       </c>
@@ -1608,7 +1620,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1774,7 +1786,7 @@
       <c r="BC2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BD2" s="12" t="s">
         <v>39</v>
       </c>
       <c r="BE2" s="6" t="s">
@@ -1823,7 +1835,7 @@
         <v>203</v>
       </c>
       <c r="BT2" s="7" t="s">
-        <v>113</v>
+        <v>269</v>
       </c>
       <c r="BU2" s="7" t="s">
         <v>214</v>
@@ -1876,8 +1888,17 @@
       <c r="CK2" s="7" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL2" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="CM2" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="CN2" s="17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2145,8 +2166,17 @@
       <c r="CK3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL3" t="s">
+        <v>2</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>2</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2414,8 +2444,17 @@
       <c r="CK4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL4" t="s">
+        <v>3</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>3</v>
+      </c>
+      <c r="CN4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2680,8 +2719,17 @@
       <c r="CK5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL5" t="s">
+        <v>4</v>
+      </c>
+      <c r="CM5" t="s">
+        <v>4</v>
+      </c>
+      <c r="CN5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2946,8 +2994,17 @@
       <c r="CK6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL6" t="s">
+        <v>5</v>
+      </c>
+      <c r="CM6" t="s">
+        <v>5</v>
+      </c>
+      <c r="CN6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3203,8 +3260,17 @@
       <c r="CK7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL7" t="s">
+        <v>7</v>
+      </c>
+      <c r="CM7" t="s">
+        <v>6</v>
+      </c>
+      <c r="CN7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3439,8 +3505,17 @@
       <c r="CK8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL8" t="s">
+        <v>6</v>
+      </c>
+      <c r="CM8" t="s">
+        <v>7</v>
+      </c>
+      <c r="CN8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3654,8 +3729,14 @@
       <c r="CK9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL9" t="s">
+        <v>8</v>
+      </c>
+      <c r="CM9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3854,8 +3935,14 @@
       <c r="CK10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL10" t="s">
+        <v>9</v>
+      </c>
+      <c r="CM10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4045,8 +4132,14 @@
       <c r="CJ11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL11" t="s">
+        <v>10</v>
+      </c>
+      <c r="CM11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -4221,8 +4314,14 @@
       <c r="CJ12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL12" t="s">
+        <v>11</v>
+      </c>
+      <c r="CM12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -4379,8 +4478,14 @@
       <c r="CJ13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL13" t="s">
+        <v>12</v>
+      </c>
+      <c r="CM13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4534,8 +4639,14 @@
       <c r="CJ14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CL14" t="s">
+        <v>13</v>
+      </c>
+      <c r="CM14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -4680,8 +4791,11 @@
       <c r="CJ15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:89" x14ac:dyDescent="0.3">
+      <c r="CM15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:92" x14ac:dyDescent="0.3">
       <c r="P16" t="s">
         <v>14</v>
       </c>

</xml_diff>